<commit_message>
Checked 1-7 assembled after restarting kernel.
</commit_message>
<xml_diff>
--- a/HeroesOfPymoli/3_Gender_Demographics.xlsx
+++ b/HeroesOfPymoli/3_Gender_Demographics.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,79 +367,33 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Gender</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Purchase Count</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Average Purchase Price</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total Purchase Value</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Avg Total Purchase per Person</t>
+          <t>Percentage of Players</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>113</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>$3.20</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>$361.94</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>$3.20</t>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>83.59%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>652</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>$3.02</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>$1,967.64</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>$3.02</t>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>14.49%</t>
         </is>
       </c>
     </row>
@@ -449,22 +403,9 @@
           <t>Other / Non-Disclosed</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>15</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>$3.35</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>$50.19</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>$3.35</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.92%</t>
         </is>
       </c>
     </row>

</xml_diff>